<commit_message>
Allow generating multiple TeasuryData in single excel
</commit_message>
<xml_diff>
--- a/bs_int/rates/quant_assessment_template.xlsx
+++ b/bs_int/rates/quant_assessment_template.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Treasury Example (with Math)" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="sheet" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="hUFFOXWFsyfPmUQYXHR06ccqnPbpBhNs3NWv3BtWhdk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="A80cp+IgUcCWxmt1pIYQwQHo/b7x3irTJxGNM5atHoo="/>
     </ext>
   </extLst>
 </workbook>
@@ -330,292 +330,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:rPr>
-              <a:t>Par and Zero</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Treasury Example (with Math)'!$K$2</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="4472C4"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Treasury Example (with Math)'!$J$3:$J$351</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Treasury Example (with Math)'!$K$3:$K$351</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Treasury Example (with Math)'!$L$2</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="ED7D31"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Treasury Example (with Math)'!$J$3:$J$351</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Treasury Example (with Math)'!$L$3:$L$351</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="2145509291"/>
-        <c:axId val="624031800"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="2145509291"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t>Month</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:spPr/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="624031800"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="624031800"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2145509291"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="5010150" cy="2695575"/>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1687990111" name="Chart 1" title="Chart"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>